<commit_message>
Commit Report, add mobile API
</commit_message>
<xml_diff>
--- a/Document/ClassDiagram/ClassExplanation.xlsx
+++ b/Document/ClassDiagram/ClassExplanation.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\11Capstone\Document\ClassDiagram\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
@@ -31,7 +26,7 @@
     <sheet name="Option" sheetId="16" r:id="rId17"/>
     <sheet name="Answer" sheetId="17" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -546,7 +541,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -578,7 +573,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -717,12 +712,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -735,6 +724,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -826,7 +821,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -861,7 +856,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1038,7 +1033,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1048,23 +1043,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.75" customWidth="1"/>
-    <col min="2" max="2" width="45.25" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-    </row>
-    <row r="2" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1072,136 +1067,136 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="48" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:2" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="48" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:2" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+    <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1241,54 +1236,54 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD6"/>
+      <selection activeCell="D3" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1305,79 +1300,79 @@
       <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1391,54 +1386,54 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1455,247 +1450,247 @@
       <selection sqref="A1:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="B4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="B12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="B13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="B14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="8" t="s">
+      <c r="B15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="B16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="8" t="s">
+      <c r="B17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1712,65 +1707,65 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1787,65 +1782,65 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1859,124 +1854,124 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C8"/>
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="B7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="B8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1993,79 +1988,79 @@
       <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="B4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2080,96 +2075,96 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="B3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="B6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2183,182 +2178,182 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D12"/>
+      <selection activeCell="D13" sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="B6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="B7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="B12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2372,54 +2367,54 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D3" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2436,51 +2431,51 @@
       <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2494,68 +2489,68 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection activeCell="D4" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="B4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2572,51 +2567,51 @@
       <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2630,82 +2625,82 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="D5" sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.875" customWidth="1"/>
-    <col min="4" max="4" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2720,82 +2715,82 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="D5" sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2812,93 +2807,93 @@
       <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="B6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>